<commit_message>
Repo updated; Project Diary erweitert
</commit_message>
<xml_diff>
--- a/Documents/Sprints/Sprint_Review_Protocol_5_Group01.xlsx
+++ b/Documents/Sprints/Sprint_Review_Protocol_5_Group01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Semester3\LVs\INNOLAB\Repo\Projekt\Git-Game\Documents\Sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511B72A9-1611-458C-9E07-AD431B1DC4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2924FA-68BC-4186-A430-5B2A5878CD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="30270" yWindow="2370" windowWidth="21600" windowHeight="11385" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -116,7 +116,10 @@
     <t>PW-Rücksetzung per Mail</t>
   </si>
   <si>
-    <t>Password wird nicht gehasht eingespeichert, wenn man sich einloggen will; 70/80% Fertig</t>
+    <t>Dashboard öffnet sich nicht, wenn man sich einloggen will; 70/80% Fertig</t>
+  </si>
+  <si>
+    <t>12.01.2022, 20:00</t>
   </si>
 </sst>
 </file>
@@ -368,6 +371,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -386,18 +407,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -414,21 +432,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -747,47 +750,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3C726-37E9-451B-9308-D99ECF6E7468}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -798,132 +801,132 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="18">
+      <c r="B4" s="21"/>
+      <c r="C4" s="22">
         <v>5</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="30">
-        <v>44573</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="20">
+      <c r="B6" s="13"/>
+      <c r="C6" s="25">
         <v>1</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -949,7 +952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -972,7 +975,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>2</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1007,7 +1010,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1017,7 +1020,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1027,7 +1030,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1037,7 +1040,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1047,7 +1050,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1057,7 +1060,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1067,7 +1070,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1080,7 +1083,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f>COUNT(A16:A25)</f>
         <v>2</v>
@@ -1102,24 +1105,19 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1134,6 +1132,11 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>